<commit_message>
extent steps and data provide
</commit_message>
<xml_diff>
--- a/src/main/java/resources/Book1.xlsx
+++ b/src/main/java/resources/Book1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10092" windowHeight="1440"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10500" windowHeight="6660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,19 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t>Testcases</t>
-  </si>
-  <si>
-    <t>Data1</t>
-  </si>
-  <si>
-    <t>Data2</t>
-  </si>
-  <si>
-    <t>Data3</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Login</t>
   </si>
@@ -51,25 +39,25 @@
     <t>logidat2</t>
   </si>
   <si>
-    <t>logidat3</t>
-  </si>
-  <si>
     <t>Purchase1</t>
   </si>
   <si>
     <t>Purchase2</t>
   </si>
   <si>
-    <t>Purchase3</t>
-  </si>
-  <si>
     <t>Checkout1</t>
   </si>
   <si>
     <t>Checkout2</t>
   </si>
   <si>
-    <t>Checkout3</t>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>postcode</t>
   </si>
 </sst>
 </file>
@@ -390,68 +378,56 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
       <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>